<commit_message>
CSV Parsing Utils TestCases -> bumped up LineCoverage to 90%
</commit_message>
<xml_diff>
--- a/src/main/resources/TestCargoDetails.xlsx
+++ b/src/main/resources/TestCargoDetails.xlsx
@@ -8,19 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abhimanyuchauhan/runner_shipment_service/src/main/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B19FCFA5-22CC-2548-BD2F-432B02E5DFAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A08707C-F70A-2542-8F76-431F6D841649}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="760" windowWidth="34560" windowHeight="20400" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CargoDetails" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="92">
   <si>
     <t>Guid</t>
   </si>
@@ -287,6 +300,15 @@
   </si>
   <si>
     <t>ABCD</t>
+  </si>
+  <si>
+    <t>IND</t>
+  </si>
+  <si>
+    <t>CG</t>
+  </si>
+  <si>
+    <t>HEG</t>
   </si>
 </sst>
 </file>
@@ -660,15 +682,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AX3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="211" workbookViewId="0">
+      <selection activeCell="V4" sqref="V4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="34.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.83203125" customWidth="1"/>
     <col min="4" max="4" width="9" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.5" bestFit="1" customWidth="1"/>
@@ -879,7 +901,7 @@
         <v>51</v>
       </c>
       <c r="D2" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="E2" t="s">
         <v>53</v>
@@ -933,13 +955,13 @@
         <v>62</v>
       </c>
       <c r="V2" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="W2" t="s">
         <v>54</v>
       </c>
       <c r="X2" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="Y2" t="s">
         <v>80</v>
@@ -1008,7 +1030,7 @@
         <v>54</v>
       </c>
       <c r="AU2" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="AV2" t="s">
         <v>54</v>
@@ -1076,19 +1098,19 @@
         <v>54</v>
       </c>
       <c r="T3" t="s">
-        <v>54</v>
+        <v>79</v>
       </c>
       <c r="U3" t="s">
         <v>73</v>
       </c>
       <c r="V3" t="s">
-        <v>59</v>
+        <v>91</v>
       </c>
       <c r="W3" t="s">
         <v>54</v>
       </c>
       <c r="X3" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="Y3" t="s">
         <v>54</v>
@@ -1157,7 +1179,7 @@
         <v>54</v>
       </c>
       <c r="AU3" t="s">
-        <v>59</v>
+        <v>90</v>
       </c>
       <c r="AV3" t="s">
         <v>54</v>

</xml_diff>